<commit_message>
REPORTGEN-709: fix issue, propose new name for report and update NIST report
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/NIST-SP800-53R4 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/NIST-SP800-53R4 Full Detailed Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB36151F-EDEA-4444-9FCC-81F5F06DFE98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FEDC64-1BB3-4D1F-8E62-67F917C88151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Application Name:</t>
   </si>
@@ -85,45 +85,24 @@
     <t>RepGen:TEXT;METRIC_TECHNICAL_DEBT</t>
   </si>
   <si>
-    <t>RepGen:TABLE;TECHNICAL_SIZING</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TECHNO_LOC</t>
-  </si>
-  <si>
     <t>Application characteristics</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=NIST-SP-800-53R4,MORE=true</t>
-  </si>
-  <si>
     <t>Findings summary for CAST under NIST-SP800-53R4</t>
   </si>
   <si>
     <t>NIST-SP800-53R4 Compliance details</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-AC</t>
-  </si>
-  <si>
     <t>CAST findings for NIST SP800 53R4 Access Control</t>
   </si>
   <si>
     <t>CAST findings details for NIST SP800 53R4 Access Control</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-AC,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings for NIST SP800 53R4 Audit and Accountability Controls</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-AU</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-AU,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings details for NIST SP800 53R4 Audit and Accountability Controls</t>
   </si>
   <si>
@@ -133,30 +112,12 @@
     <t>CAST findings details for NIST SP800 53R4 Security Assessment and Authorization Controls</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-CA,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-CA</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-CM</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-CM,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings details for NIST SP800 53R4 Configuration Management Controls</t>
   </si>
   <si>
     <t>CAST findings for NIST SP800 53R4 Configuration Management Controls</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-IA</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-IA,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings details for NIST SP800 53R4 Identification and Authentication Controls</t>
   </si>
   <si>
@@ -169,34 +130,130 @@
     <t>CAST findings for NIST SP800 53R4 System and Service Acquisitions Controls</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-SA,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SA</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SC</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-SC,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings details for NIST SP800 53R4 System and Communication Protection Controls</t>
   </si>
   <si>
     <t>CAST findings for NIST SP800 53R4 System and Communication Protection Controls</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SI</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=NIST-SP-800-53R4-SI,COUNT=-1</t>
-  </si>
-  <si>
     <t>CAST findings details for NIST SP800 53R4 System and Information Integrity Controls</t>
   </si>
   <si>
     <t>CAST findings for NIST SP800 53R4 System and Information Integrity Controls</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNO_LOC;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNICAL_SIZING;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Quality Standard</t>
+  </si>
+  <si>
+    <t>Total Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Added Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Removed Vulnerabilities</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=NIST-SP-800-53R4,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-AC,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>Object Type</t>
+  </si>
+  <si>
+    <t>Violation Status</t>
+  </si>
+  <si>
+    <t>Associated Value</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Start Line</t>
+  </si>
+  <si>
+    <t>End Line</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-AC,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-AU,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-AU,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-CA,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-CA,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-CM,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-CM,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-IA,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-IA,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SA,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-SA,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SC,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-SC,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=NIST-SP-800-53R4-SI,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=NIST-SP-800-53R4-SI,COUNT=-1,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -403,7 +460,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -473,6 +530,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -850,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O13"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,7 +951,7 @@
     </row>
     <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -929,27 +996,59 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D9" s="26"/>
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -966,9 +1065,495 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7E084B-1D41-49A1-AAE8-65E5FD99EAE8}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="88.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" customWidth="1"/>
+    <col min="7" max="7" width="37.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60019302-308A-442F-B9EA-3F649E847332}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6184CFD3-505D-44C0-8258-50A02CF4F83B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68947EEB-3915-46CA-938B-9EF94DC11C5F}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40429C24-E986-40B1-9C54-93D6527149C0}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.109375" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="7" max="7" width="58" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EB8EA9-CBE4-4B5D-A35C-7E148B322568}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398772F4-1EC0-446D-8794-6788C8DEC765}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="86.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E33A766-BEF1-4CAD-9B15-BE530492E644}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="100.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -976,18 +1561,44 @@
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -995,28 +1606,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60019302-308A-442F-B9EA-3F649E847332}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00038B0F-4F74-4ACF-8A7F-FE15A067CF76}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="100.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1025,9 +1668,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6184CFD3-505D-44C0-8258-50A02CF4F83B}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C28B7BF-B505-460E-B5F5-CEF317C8DA21}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1039,18 +1682,44 @@
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1"/>
+    <col min="6" max="6" width="50.44140625" customWidth="1"/>
+    <col min="7" max="7" width="50.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1058,28 +1727,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68947EEB-3915-46CA-938B-9EF94DC11C5F}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8D923-188E-4CB6-BF7E-B970F3C6E30D}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="100.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1088,12 +1789,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40429C24-E986-40B1-9C54-93D6527149C0}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79906E84-4B34-4770-9305-4F2F91D7EFE1}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC577CBB-D408-44A0-A911-378AA65DFFF8}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="100.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB41B1C-9240-4348-9FC9-45CED54B99B9}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,19 +1923,45 @@
     <col min="1" max="1" width="88.21875" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.5546875" customWidth="1"/>
+    <col min="6" max="6" width="47.77734375" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>40</v>
       </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,335 +1969,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EB8EA9-CBE4-4B5D-A35C-7E148B322568}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398772F4-1EC0-446D-8794-6788C8DEC765}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E33A766-BEF1-4CAD-9B15-BE530492E644}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEDA8E1-603E-4AFF-9626-7A5FC25447BA}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="100.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00038B0F-4F74-4ACF-8A7F-FE15A067CF76}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C28B7BF-B505-460E-B5F5-CEF317C8DA21}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8D923-188E-4CB6-BF7E-B970F3C6E30D}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79906E84-4B34-4770-9305-4F2F91D7EFE1}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC577CBB-D408-44A0-A911-378AA65DFFF8}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB41B1C-9240-4348-9FC9-45CED54B99B9}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEDA8E1-603E-4AFF-9626-7A5FC25447BA}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>29</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>